<commit_message>
Ajout photos résultats au readme
</commit_message>
<xml_diff>
--- a/ResultatsBancTest/Flex.xlsx
+++ b/ResultatsBancTest/Flex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louis-maxencehotton/Desktop/ProjetCapteurGraphite2022-LM-TL/ResultatsBancTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6864ACA8-7309-5742-A6EC-87212E11BDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D30D456-9DF6-774A-80FA-11E221BB842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{786922CB-4535-4135-98E9-A5AD90371A33}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{786922CB-4535-4135-98E9-A5AD90371A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -227,13 +227,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.7314523184601924E-2"/>
-                  <c:y val="-0.29862605715952173"/>
+                  <c:x val="-0.18859551288965593"/>
+                  <c:y val="-6.8028895470634981E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1645,7 +1646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898D8742-97F4-44FD-B2D3-C2BB3A655711}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>

</xml_diff>